<commit_message>
Updated Raw Data with carbon intensity values
</commit_message>
<xml_diff>
--- a/Raw Data.xlsx
+++ b/Raw Data.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LENOVO\OneDrive - University of Nottingham Malaysia\The University of Nottingham\BC COP26 Trilateral Research Initiative\BCCOP26TrilateralProject\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://numcmy-my.sharepoint.com/personal/ebxps1_nottingham_edu_my/Documents/.tmp.drivedownload/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD358DB1-D024-4DFC-A7DE-680B6F2C694D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="16" documentId="13_ncr:1_{DD358DB1-D024-4DFC-A7DE-680B6F2C694D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{729DD6C3-2519-402D-A67E-E7881F66F63C}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="3" xr2:uid="{6BC639D9-110C-4E54-A662-BDDB0F5A7A64}"/>
+    <workbookView minimized="1" xWindow="4020" yWindow="3045" windowWidth="15375" windowHeight="7875" activeTab="3" xr2:uid="{6BC639D9-110C-4E54-A662-BDDB0F5A7A64}"/>
   </bookViews>
   <sheets>
     <sheet name="Period 1" sheetId="1" r:id="rId1"/>
@@ -229,7 +229,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -243,6 +243,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -252,10 +258,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -920,7 +923,7 @@
   <dimension ref="A1:I40"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="C38" sqref="C38"/>
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -929,21 +932,21 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="B1" s="6"/>
-      <c r="C1" s="7"/>
-      <c r="D1" s="5" t="s">
+      <c r="B1" s="8"/>
+      <c r="C1" s="9"/>
+      <c r="D1" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="E1" s="6"/>
-      <c r="F1" s="7"/>
-      <c r="G1" s="5" t="s">
+      <c r="E1" s="8"/>
+      <c r="F1" s="9"/>
+      <c r="G1" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="H1" s="6"/>
-      <c r="I1" s="7"/>
+      <c r="H1" s="8"/>
+      <c r="I1" s="9"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
@@ -952,18 +955,27 @@
       <c r="B2" s="1">
         <v>18</v>
       </c>
+      <c r="C2" s="1">
+        <v>0</v>
+      </c>
       <c r="D2" s="1" t="s">
         <v>0</v>
       </c>
       <c r="E2" s="1">
         <v>30</v>
       </c>
+      <c r="F2" s="1">
+        <v>0</v>
+      </c>
       <c r="G2" s="1" t="s">
         <v>0</v>
       </c>
       <c r="H2" s="1">
         <v>40</v>
       </c>
+      <c r="I2" s="1">
+        <v>0</v>
+      </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
@@ -972,17 +984,26 @@
       <c r="B3" s="1">
         <v>19.2</v>
       </c>
+      <c r="C3" s="1">
+        <v>0.5</v>
+      </c>
       <c r="D3" s="1" t="s">
         <v>13</v>
       </c>
       <c r="E3" s="1">
         <v>30</v>
       </c>
+      <c r="F3" s="1">
+        <v>0.5</v>
+      </c>
       <c r="G3" s="1" t="s">
         <v>13</v>
       </c>
       <c r="H3" s="1">
         <v>40</v>
+      </c>
+      <c r="I3" s="1">
+        <v>0.5</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
@@ -992,18 +1013,27 @@
       <c r="B4" s="1">
         <v>6</v>
       </c>
+      <c r="C4" s="1">
+        <v>0.8</v>
+      </c>
       <c r="D4" s="1" t="s">
         <v>2</v>
       </c>
       <c r="E4" s="1">
         <v>5</v>
       </c>
+      <c r="F4" s="1">
+        <v>0.8</v>
+      </c>
       <c r="G4" s="1" t="s">
         <v>2</v>
       </c>
       <c r="H4" s="1">
         <v>5</v>
       </c>
+      <c r="I4" s="1">
+        <v>0.8</v>
+      </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
@@ -1012,17 +1042,26 @@
       <c r="B5" s="1">
         <v>16.8</v>
       </c>
+      <c r="C5" s="1">
+        <v>1</v>
+      </c>
       <c r="D5" s="1" t="s">
         <v>3</v>
       </c>
       <c r="E5" s="1">
         <v>10</v>
       </c>
+      <c r="F5" s="1">
+        <v>1</v>
+      </c>
       <c r="G5" s="1" t="s">
         <v>3</v>
       </c>
       <c r="H5" s="1">
         <v>5</v>
+      </c>
+      <c r="I5" s="1">
+        <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1033,6 +1072,10 @@
         <f>SUM(B2:B5)</f>
         <v>60</v>
       </c>
+      <c r="C6" s="3">
+        <f>(B2*C2)+(B3*C3)+(B4*C4)+(B5*C5)</f>
+        <v>31.200000000000003</v>
+      </c>
       <c r="D6" s="3" t="s">
         <v>14</v>
       </c>
@@ -1040,12 +1083,20 @@
         <f>SUM(E2:E5)</f>
         <v>75</v>
       </c>
+      <c r="F6" s="10">
+        <f>(E2*F2)+(E3*F3)+(E4*F4)+(E5*F5)</f>
+        <v>29</v>
+      </c>
       <c r="G6" s="3" t="s">
         <v>14</v>
       </c>
       <c r="H6" s="3">
         <f>SUM(H2:H5)</f>
         <v>90</v>
+      </c>
+      <c r="I6" s="10">
+        <f>(H2*I2)+(H3*I3)+(H4*I4)+(H5*I5)</f>
+        <v>29</v>
       </c>
     </row>
     <row r="7" spans="1:9" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
@@ -1347,58 +1398,58 @@
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A25" s="8" t="s">
+      <c r="A25" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="B25" s="8">
+      <c r="B25" s="5">
         <v>6</v>
       </c>
-      <c r="C25" s="9">
+      <c r="C25" s="6">
         <v>0.53</v>
       </c>
-      <c r="D25" s="9" t="s">
+      <c r="D25" s="6" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A26" s="8" t="s">
+      <c r="A26" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="B26" s="8">
+      <c r="B26" s="5">
         <v>8</v>
       </c>
-      <c r="C26" s="8">
+      <c r="C26" s="5">
         <v>8</v>
       </c>
-      <c r="D26" s="9" t="s">
+      <c r="D26" s="6" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A27" s="8" t="s">
+      <c r="A27" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="B27" s="8">
-        <v>5</v>
-      </c>
-      <c r="C27" s="8">
-        <v>5</v>
-      </c>
-      <c r="D27" s="9" t="s">
+      <c r="B27" s="5">
+        <v>5</v>
+      </c>
+      <c r="C27" s="5">
+        <v>5</v>
+      </c>
+      <c r="D27" s="6" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A28" s="8" t="s">
+      <c r="A28" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="B28" s="8">
+      <c r="B28" s="5">
         <v>3.8</v>
       </c>
-      <c r="C28" s="8">
+      <c r="C28" s="5">
         <v>3.8</v>
       </c>
-      <c r="D28" s="9" t="s">
+      <c r="D28" s="6" t="s">
         <v>3</v>
       </c>
     </row>
@@ -1472,58 +1523,58 @@
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A37" s="8" t="s">
+      <c r="A37" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="B37" s="8">
+      <c r="B37" s="5">
         <v>6</v>
       </c>
-      <c r="C37" s="9">
+      <c r="C37" s="6">
         <v>4.43</v>
       </c>
-      <c r="D37" s="9" t="s">
+      <c r="D37" s="6" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A38" s="8" t="s">
+      <c r="A38" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="B38" s="8">
+      <c r="B38" s="5">
         <v>8</v>
       </c>
-      <c r="C38" s="8">
+      <c r="C38" s="5">
         <v>8</v>
       </c>
-      <c r="D38" s="9" t="s">
+      <c r="D38" s="6" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A39" s="8" t="s">
+      <c r="A39" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="B39" s="8">
-        <v>5</v>
-      </c>
-      <c r="C39" s="8">
-        <v>5</v>
-      </c>
-      <c r="D39" s="9" t="s">
+      <c r="B39" s="5">
+        <v>5</v>
+      </c>
+      <c r="C39" s="5">
+        <v>5</v>
+      </c>
+      <c r="D39" s="6" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A40" s="8" t="s">
+      <c r="A40" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="B40" s="8">
+      <c r="B40" s="5">
         <v>3.8</v>
       </c>
-      <c r="C40" s="8">
+      <c r="C40" s="5">
         <v>3.8</v>
       </c>
-      <c r="D40" s="9" t="s">
+      <c r="D40" s="6" t="s">
         <v>3</v>
       </c>
     </row>

</xml_diff>